<commit_message>
Att add conect postgres
</commit_message>
<xml_diff>
--- a/Planilhas/População ESTADUAL.xlsx
+++ b/Planilhas/População ESTADUAL.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,25 +446,20 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>id_produto</t>
+          <t>Categoria</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Categoria</t>
+          <t>População</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>População</t>
+          <t>unidade</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>unidade</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>ano</t>
         </is>
@@ -483,23 +478,20 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>1581196</v>
+          <t>1581196</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F2" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -518,23 +510,20 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>830018</v>
+          <t>830018</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F3" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -553,23 +542,20 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>3941613</v>
+          <t>3941613</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F4" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -588,23 +574,20 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>636707</v>
+          <t>636707</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F5" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -623,23 +606,20 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>8120131</v>
+          <t>8120131</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F6" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -658,23 +638,20 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>733759</v>
+          <t>733759</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F7" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -693,23 +670,20 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>1511460</v>
+          <t>1511460</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F8" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -728,23 +702,20 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>6776699</v>
+          <t>6776699</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F9" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -763,23 +734,20 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>3271199</v>
+          <t>3271199</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F10" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -798,23 +766,20 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>8794957</v>
+          <t>8794957</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F11" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -833,23 +798,20 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>3302729</v>
+          <t>3302729</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F12" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -868,23 +830,20 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>3974687</v>
+          <t>3974687</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F13" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -903,23 +862,20 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>9058931</v>
+          <t>9058931</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F14" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -938,23 +894,20 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>3127683</v>
+          <t>3127683</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F15" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -973,23 +926,20 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>2210004</v>
+          <t>2210004</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F16" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -1008,23 +958,20 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>14141626</v>
+          <t>14141626</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F17" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -1043,23 +990,20 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>20539989</v>
+          <t>20539989</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F18" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -1078,23 +1022,20 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>3833712</v>
+          <t>3833712</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F19" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -1113,23 +1054,20 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
-        <v>16055174</v>
+          <t>16055174</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F20" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -1148,23 +1086,20 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>44411238</v>
+          <t>44411238</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F21" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -1183,23 +1118,20 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
-        <v>11444380</v>
+          <t>11444380</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F22" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -1218,23 +1150,20 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E23" t="n">
-        <v>7610361</v>
+          <t>7610361</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F23" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -1253,23 +1182,20 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E24" t="n">
-        <v>10882965</v>
+          <t>10882965</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F24" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -1288,23 +1214,20 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E25" t="n">
-        <v>2757013</v>
+          <t>2757013</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F25" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -1323,23 +1246,20 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E26" t="n">
-        <v>3658649</v>
+          <t>3658649</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F26" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -1358,23 +1278,20 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E27" t="n">
-        <v>7056495</v>
+          <t>7056495</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F27" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>
@@ -1393,23 +1310,20 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E28" t="n">
-        <v>2817381</v>
+          <t>2817381</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
       </c>
       <c r="F28" t="inlineStr">
-        <is>
-          <t>Pessoas</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
         <is>
           <t>01/01/2022</t>
         </is>

</xml_diff>